<commit_message>
Update life expectancy, readme and IMR name
</commit_message>
<xml_diff>
--- a/data/meta/G77 and OECD countries.xlsx
+++ b/data/meta/G77 and OECD countries.xlsx
@@ -41,6 +41,9 @@
     <t>Entity</t>
   </si>
   <si>
+    <t>not used yet</t>
+  </si>
+  <si>
     <t>Group</t>
   </si>
   <si>
@@ -341,6 +344,12 @@
     <t>Saint Vincent and the Grenadines</t>
   </si>
   <si>
+    <t>VERSION</t>
+  </si>
+  <si>
+    <t>COLOR_CATEGORIES_1_EN</t>
+  </si>
+  <si>
     <t>Samoa</t>
   </si>
   <si>
@@ -831,15 +840,6 @@
   </si>
   <si>
     <t>Yugoslavia</t>
-  </si>
-  <si>
-    <t>not used yet</t>
-  </si>
-  <si>
-    <t>VERSION</t>
-  </si>
-  <si>
-    <t>COLOR_CATEGORIES_1_EN</t>
   </si>
 </sst>
 </file>
@@ -990,19 +990,19 @@
 </styleSheet>
 </file>
 
-<file path=xl/drawings/worksheetdrawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
 </file>
 
-<file path=xl/drawings/worksheetdrawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
 </file>
 
-<file path=xl/drawings/worksheetdrawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
 </file>
 
-<file path=xl/drawings/worksheetdrawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
 </file>
 
@@ -3642,7 +3642,7 @@
         <v>7</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C1" s="10"/>
       <c r="D1" s="3"/>
@@ -3666,10 +3666,10 @@
     </row>
     <row r="2">
       <c r="A2" s="11" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
@@ -3693,10 +3693,10 @@
     </row>
     <row r="3">
       <c r="A3" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="12" t="s">
         <v>11</v>
-      </c>
-      <c r="B3" s="12" t="s">
-        <v>10</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
@@ -3720,10 +3720,10 @@
     </row>
     <row r="4">
       <c r="A4" s="11" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
@@ -3747,10 +3747,10 @@
     </row>
     <row r="5">
       <c r="A5" s="11" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C5" s="13"/>
       <c r="D5" s="13"/>
@@ -3774,10 +3774,10 @@
     </row>
     <row r="6">
       <c r="A6" s="11" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C6" s="13"/>
       <c r="D6" s="13"/>
@@ -3801,10 +3801,10 @@
     </row>
     <row r="7">
       <c r="A7" s="11" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C7" s="13"/>
       <c r="D7" s="13"/>
@@ -3828,10 +3828,10 @@
     </row>
     <row r="8">
       <c r="A8" s="11" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C8" s="13"/>
       <c r="D8" s="13"/>
@@ -3855,10 +3855,10 @@
     </row>
     <row r="9">
       <c r="A9" s="11" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C9" s="13"/>
       <c r="D9" s="13"/>
@@ -3882,10 +3882,10 @@
     </row>
     <row r="10">
       <c r="A10" s="11" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C10" s="13"/>
       <c r="D10" s="13"/>
@@ -3909,10 +3909,10 @@
     </row>
     <row r="11">
       <c r="A11" s="11" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C11" s="13"/>
       <c r="D11" s="13"/>
@@ -3936,10 +3936,10 @@
     </row>
     <row r="12">
       <c r="A12" s="11" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B12" s="12" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C12" s="13"/>
       <c r="D12" s="13"/>
@@ -3963,10 +3963,10 @@
     </row>
     <row r="13">
       <c r="A13" s="11" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B13" s="12" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C13" s="13"/>
       <c r="D13" s="13"/>
@@ -3990,10 +3990,10 @@
     </row>
     <row r="14">
       <c r="A14" s="11" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C14" s="13"/>
       <c r="D14" s="13"/>
@@ -4017,10 +4017,10 @@
     </row>
     <row r="15">
       <c r="A15" s="11" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B15" s="12" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C15" s="14"/>
       <c r="D15" s="14"/>
@@ -4044,10 +4044,10 @@
     </row>
     <row r="16">
       <c r="A16" s="11" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B16" s="12" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C16" s="14"/>
       <c r="D16" s="15"/>
@@ -4071,10 +4071,10 @@
     </row>
     <row r="17">
       <c r="A17" s="11" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B17" s="12" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C17" s="14"/>
       <c r="D17" s="14"/>
@@ -4098,10 +4098,10 @@
     </row>
     <row r="18">
       <c r="A18" s="11" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B18" s="12" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C18" s="14"/>
       <c r="D18" s="14"/>
@@ -4125,10 +4125,10 @@
     </row>
     <row r="19">
       <c r="A19" s="11" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B19" s="12" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C19" s="14"/>
       <c r="D19" s="14"/>
@@ -4152,10 +4152,10 @@
     </row>
     <row r="20">
       <c r="A20" s="11" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B20" s="12" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C20" s="14"/>
       <c r="D20" s="14"/>
@@ -4179,10 +4179,10 @@
     </row>
     <row r="21">
       <c r="A21" s="11" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B21" s="12" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C21" s="14"/>
       <c r="D21" s="14"/>
@@ -4206,10 +4206,10 @@
     </row>
     <row r="22">
       <c r="A22" s="11" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B22" s="12" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C22" s="14"/>
       <c r="D22" s="14"/>
@@ -4233,10 +4233,10 @@
     </row>
     <row r="23">
       <c r="A23" s="11" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B23" s="12" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C23" s="14"/>
       <c r="D23" s="14"/>
@@ -4260,10 +4260,10 @@
     </row>
     <row r="24">
       <c r="A24" s="11" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B24" s="12" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C24" s="14"/>
       <c r="D24" s="14"/>
@@ -4287,10 +4287,10 @@
     </row>
     <row r="25">
       <c r="A25" s="11" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B25" s="12" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C25" s="14"/>
       <c r="D25" s="14"/>
@@ -4314,10 +4314,10 @@
     </row>
     <row r="26">
       <c r="A26" s="11" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B26" s="12" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C26" s="14"/>
       <c r="D26" s="14"/>
@@ -4341,10 +4341,10 @@
     </row>
     <row r="27">
       <c r="A27" s="11" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B27" s="12" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C27" s="14"/>
       <c r="D27" s="14"/>
@@ -4368,10 +4368,10 @@
     </row>
     <row r="28">
       <c r="A28" s="11" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B28" s="12" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C28" s="14"/>
       <c r="D28" s="14"/>
@@ -4395,10 +4395,10 @@
     </row>
     <row r="29">
       <c r="A29" s="11" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B29" s="12" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C29" s="14"/>
       <c r="D29" s="14"/>
@@ -4422,10 +4422,10 @@
     </row>
     <row r="30">
       <c r="A30" s="11" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B30" s="12" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C30" s="14"/>
       <c r="D30" s="14"/>
@@ -4449,10 +4449,10 @@
     </row>
     <row r="31">
       <c r="A31" s="11" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B31" s="12" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C31" s="14"/>
       <c r="D31" s="14"/>
@@ -4476,10 +4476,10 @@
     </row>
     <row r="32">
       <c r="A32" s="11" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B32" s="12" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C32" s="14"/>
       <c r="D32" s="16"/>
@@ -4503,10 +4503,10 @@
     </row>
     <row r="33">
       <c r="A33" s="11" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B33" s="12" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C33" s="14"/>
       <c r="D33" s="14"/>
@@ -4530,10 +4530,10 @@
     </row>
     <row r="34">
       <c r="A34" s="11" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B34" s="12" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C34" s="14"/>
       <c r="D34" s="14"/>
@@ -4557,10 +4557,10 @@
     </row>
     <row r="35">
       <c r="A35" s="11" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B35" s="12" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C35" s="14"/>
       <c r="D35" s="14"/>
@@ -4584,10 +4584,10 @@
     </row>
     <row r="36">
       <c r="A36" s="11" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B36" s="12" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C36" s="14"/>
       <c r="D36" s="14"/>
@@ -4611,10 +4611,10 @@
     </row>
     <row r="37">
       <c r="A37" s="11" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B37" s="12" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C37" s="14"/>
       <c r="D37" s="14"/>
@@ -4638,10 +4638,10 @@
     </row>
     <row r="38">
       <c r="A38" s="11" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B38" s="12" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C38" s="14"/>
       <c r="D38" s="14"/>
@@ -4665,10 +4665,10 @@
     </row>
     <row r="39">
       <c r="A39" s="11" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B39" s="12" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C39" s="14"/>
       <c r="D39" s="14"/>
@@ -4692,10 +4692,10 @@
     </row>
     <row r="40">
       <c r="A40" s="11" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B40" s="12" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C40" s="14"/>
       <c r="D40" s="14"/>
@@ -4719,10 +4719,10 @@
     </row>
     <row r="41">
       <c r="A41" s="11" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B41" s="12" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C41" s="14"/>
       <c r="D41" s="14"/>
@@ -4746,10 +4746,10 @@
     </row>
     <row r="42">
       <c r="A42" s="11" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B42" s="12" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C42" s="14"/>
       <c r="D42" s="14"/>
@@ -4773,10 +4773,10 @@
     </row>
     <row r="43">
       <c r="A43" s="11" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B43" s="12" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C43" s="14"/>
       <c r="D43" s="14"/>
@@ -4800,10 +4800,10 @@
     </row>
     <row r="44">
       <c r="A44" s="11" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B44" s="12" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C44" s="14"/>
       <c r="D44" s="14"/>
@@ -4827,10 +4827,10 @@
     </row>
     <row r="45">
       <c r="A45" s="11" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B45" s="12" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C45" s="14"/>
       <c r="D45" s="14"/>
@@ -4854,10 +4854,10 @@
     </row>
     <row r="46">
       <c r="A46" s="11" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B46" s="12" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C46" s="14"/>
       <c r="D46" s="14"/>
@@ -4881,10 +4881,10 @@
     </row>
     <row r="47">
       <c r="A47" s="11" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B47" s="12" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C47" s="14"/>
       <c r="D47" s="13"/>
@@ -4908,10 +4908,10 @@
     </row>
     <row r="48">
       <c r="A48" s="11" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B48" s="12" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C48" s="14"/>
       <c r="D48" s="15"/>
@@ -4935,10 +4935,10 @@
     </row>
     <row r="49">
       <c r="A49" s="11" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B49" s="12" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C49" s="14"/>
       <c r="D49" s="14"/>
@@ -4962,10 +4962,10 @@
     </row>
     <row r="50">
       <c r="A50" s="11" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B50" s="12" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C50" s="14"/>
       <c r="D50" s="14"/>
@@ -4989,10 +4989,10 @@
     </row>
     <row r="51">
       <c r="A51" s="11" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B51" s="12" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C51" s="14"/>
       <c r="D51" s="14"/>
@@ -5016,10 +5016,10 @@
     </row>
     <row r="52">
       <c r="A52" s="11" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B52" s="12" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C52" s="14"/>
       <c r="D52" s="14"/>
@@ -5043,10 +5043,10 @@
     </row>
     <row r="53">
       <c r="A53" s="11" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B53" s="12" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C53" s="14"/>
       <c r="D53" s="14"/>
@@ -5070,10 +5070,10 @@
     </row>
     <row r="54">
       <c r="A54" s="11" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B54" s="12" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C54" s="13"/>
       <c r="D54" s="13"/>
@@ -5097,10 +5097,10 @@
     </row>
     <row r="55">
       <c r="A55" s="11" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B55" s="12" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C55" s="13"/>
       <c r="D55" s="13"/>
@@ -5124,10 +5124,10 @@
     </row>
     <row r="56">
       <c r="A56" s="11" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B56" s="12" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C56" s="13"/>
       <c r="D56" s="13"/>
@@ -5151,10 +5151,10 @@
     </row>
     <row r="57">
       <c r="A57" s="11" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B57" s="12" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C57" s="13"/>
       <c r="D57" s="13"/>
@@ -5178,10 +5178,10 @@
     </row>
     <row r="58">
       <c r="A58" s="11" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B58" s="12" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C58" s="13"/>
       <c r="D58" s="13"/>
@@ -5205,10 +5205,10 @@
     </row>
     <row r="59">
       <c r="A59" s="11" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B59" s="12" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C59" s="13"/>
       <c r="D59" s="13"/>
@@ -5232,10 +5232,10 @@
     </row>
     <row r="60">
       <c r="A60" s="11" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B60" s="12" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C60" s="13"/>
       <c r="D60" s="13"/>
@@ -5259,10 +5259,10 @@
     </row>
     <row r="61">
       <c r="A61" s="11" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B61" s="12" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C61" s="13"/>
       <c r="D61" s="13"/>
@@ -5286,10 +5286,10 @@
     </row>
     <row r="62">
       <c r="A62" s="11" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B62" s="12" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C62" s="13"/>
       <c r="D62" s="13"/>
@@ -5313,10 +5313,10 @@
     </row>
     <row r="63">
       <c r="A63" s="11" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B63" s="12" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C63" s="13"/>
       <c r="D63" s="13"/>
@@ -5340,10 +5340,10 @@
     </row>
     <row r="64">
       <c r="A64" s="11" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B64" s="12" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C64" s="13"/>
       <c r="D64" s="13"/>
@@ -5367,10 +5367,10 @@
     </row>
     <row r="65">
       <c r="A65" s="11" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B65" s="12" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C65" s="13"/>
       <c r="D65" s="13"/>
@@ -5394,10 +5394,10 @@
     </row>
     <row r="66">
       <c r="A66" s="11" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B66" s="12" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C66" s="13"/>
       <c r="D66" s="13"/>
@@ -5421,10 +5421,10 @@
     </row>
     <row r="67">
       <c r="A67" s="11" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B67" s="12" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C67" s="13"/>
       <c r="D67" s="13"/>
@@ -5448,10 +5448,10 @@
     </row>
     <row r="68">
       <c r="A68" s="11" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B68" s="12" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C68" s="13"/>
       <c r="D68" s="13"/>
@@ -5475,10 +5475,10 @@
     </row>
     <row r="69">
       <c r="A69" s="11" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B69" s="12" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C69" s="13"/>
       <c r="D69" s="13"/>
@@ -5502,10 +5502,10 @@
     </row>
     <row r="70">
       <c r="A70" s="11" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B70" s="12" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C70" s="13"/>
       <c r="D70" s="13"/>
@@ -5529,10 +5529,10 @@
     </row>
     <row r="71">
       <c r="A71" s="11" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B71" s="12" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C71" s="13"/>
       <c r="D71" s="13"/>
@@ -5556,10 +5556,10 @@
     </row>
     <row r="72">
       <c r="A72" s="11" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B72" s="12" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C72" s="13"/>
       <c r="D72" s="13"/>
@@ -5583,10 +5583,10 @@
     </row>
     <row r="73">
       <c r="A73" s="11" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B73" s="12" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C73" s="13"/>
       <c r="D73" s="13"/>
@@ -5610,10 +5610,10 @@
     </row>
     <row r="74">
       <c r="A74" s="11" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B74" s="12" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C74" s="13"/>
       <c r="D74" s="13"/>
@@ -5637,10 +5637,10 @@
     </row>
     <row r="75">
       <c r="A75" s="11" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B75" s="12" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C75" s="13"/>
       <c r="D75" s="13"/>
@@ -5664,10 +5664,10 @@
     </row>
     <row r="76">
       <c r="A76" s="11" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B76" s="12" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C76" s="13"/>
       <c r="D76" s="13"/>
@@ -5691,10 +5691,10 @@
     </row>
     <row r="77">
       <c r="A77" s="11" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B77" s="12" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C77" s="13"/>
       <c r="D77" s="13"/>
@@ -5718,10 +5718,10 @@
     </row>
     <row r="78">
       <c r="A78" s="11" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B78" s="12" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C78" s="13"/>
       <c r="D78" s="13"/>
@@ -5745,10 +5745,10 @@
     </row>
     <row r="79">
       <c r="A79" s="11" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B79" s="12" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C79" s="13"/>
       <c r="D79" s="13"/>
@@ -5772,10 +5772,10 @@
     </row>
     <row r="80">
       <c r="A80" s="11" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B80" s="12" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C80" s="13"/>
       <c r="D80" s="13"/>
@@ -5799,10 +5799,10 @@
     </row>
     <row r="81">
       <c r="A81" s="11" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B81" s="12" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C81" s="13"/>
       <c r="D81" s="13"/>
@@ -5826,10 +5826,10 @@
     </row>
     <row r="82">
       <c r="A82" s="11" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B82" s="12" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C82" s="13"/>
       <c r="D82" s="13"/>
@@ -5853,10 +5853,10 @@
     </row>
     <row r="83">
       <c r="A83" s="11" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B83" s="12" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C83" s="13"/>
       <c r="D83" s="13"/>
@@ -5880,10 +5880,10 @@
     </row>
     <row r="84">
       <c r="A84" s="11" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B84" s="12" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C84" s="13"/>
       <c r="D84" s="13"/>
@@ -5907,10 +5907,10 @@
     </row>
     <row r="85">
       <c r="A85" s="11" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B85" s="12" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C85" s="13"/>
       <c r="D85" s="13"/>
@@ -5934,10 +5934,10 @@
     </row>
     <row r="86">
       <c r="A86" s="11" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B86" s="12" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C86" s="13"/>
       <c r="D86" s="13"/>
@@ -5961,10 +5961,10 @@
     </row>
     <row r="87">
       <c r="A87" s="11" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B87" s="12" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C87" s="13"/>
       <c r="D87" s="13"/>
@@ -5988,10 +5988,10 @@
     </row>
     <row r="88">
       <c r="A88" s="11" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B88" s="12" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C88" s="13"/>
       <c r="D88" s="13"/>
@@ -6015,10 +6015,10 @@
     </row>
     <row r="89">
       <c r="A89" s="11" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B89" s="12" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C89" s="13"/>
       <c r="D89" s="13"/>
@@ -6042,10 +6042,10 @@
     </row>
     <row r="90">
       <c r="A90" s="11" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B90" s="12" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C90" s="13"/>
       <c r="D90" s="13"/>
@@ -6069,10 +6069,10 @@
     </row>
     <row r="91">
       <c r="A91" s="11" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B91" s="12" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C91" s="13"/>
       <c r="D91" s="13"/>
@@ -6096,10 +6096,10 @@
     </row>
     <row r="92">
       <c r="A92" s="11" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B92" s="12" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C92" s="13"/>
       <c r="D92" s="13"/>
@@ -6123,10 +6123,10 @@
     </row>
     <row r="93">
       <c r="A93" s="11" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B93" s="12" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C93" s="13"/>
       <c r="D93" s="13"/>
@@ -6150,10 +6150,10 @@
     </row>
     <row r="94">
       <c r="A94" s="11" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B94" s="12" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C94" s="13"/>
       <c r="D94" s="13"/>
@@ -6177,10 +6177,10 @@
     </row>
     <row r="95">
       <c r="A95" s="11" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B95" s="12" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C95" s="13"/>
       <c r="D95" s="13"/>
@@ -6204,10 +6204,10 @@
     </row>
     <row r="96">
       <c r="A96" s="11" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B96" s="12" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C96" s="13"/>
       <c r="D96" s="13"/>
@@ -6231,10 +6231,10 @@
     </row>
     <row r="97">
       <c r="A97" s="11" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B97" s="12" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C97" s="13"/>
       <c r="D97" s="13"/>
@@ -6258,10 +6258,10 @@
     </row>
     <row r="98">
       <c r="A98" s="11" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B98" s="12" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C98" s="13"/>
       <c r="D98" s="13"/>
@@ -6285,10 +6285,10 @@
     </row>
     <row r="99">
       <c r="A99" s="11" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B99" s="12" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C99" s="13"/>
       <c r="D99" s="13"/>
@@ -6312,10 +6312,10 @@
     </row>
     <row r="100">
       <c r="A100" s="11" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="B100" s="12" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C100" s="13"/>
       <c r="D100" s="13"/>
@@ -6339,10 +6339,10 @@
     </row>
     <row r="101">
       <c r="A101" s="11" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="B101" s="12" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C101" s="13"/>
       <c r="D101" s="13"/>
@@ -6366,10 +6366,10 @@
     </row>
     <row r="102">
       <c r="A102" s="11" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="B102" s="12" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C102" s="13"/>
       <c r="D102" s="13"/>
@@ -6393,10 +6393,10 @@
     </row>
     <row r="103">
       <c r="A103" s="11" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="B103" s="12" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C103" s="13"/>
       <c r="D103" s="13"/>
@@ -6420,10 +6420,10 @@
     </row>
     <row r="104">
       <c r="A104" s="11" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="B104" s="12" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C104" s="13"/>
       <c r="D104" s="13"/>
@@ -6447,10 +6447,10 @@
     </row>
     <row r="105">
       <c r="A105" s="11" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="B105" s="12" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C105" s="13"/>
       <c r="D105" s="13"/>
@@ -6474,10 +6474,10 @@
     </row>
     <row r="106">
       <c r="A106" s="11" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="B106" s="12" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C106" s="13"/>
       <c r="D106" s="13"/>
@@ -6501,10 +6501,10 @@
     </row>
     <row r="107">
       <c r="A107" s="11" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="B107" s="12" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C107" s="13"/>
       <c r="D107" s="13"/>
@@ -6528,10 +6528,10 @@
     </row>
     <row r="108">
       <c r="A108" s="11" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="B108" s="12" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C108" s="13"/>
       <c r="D108" s="13"/>
@@ -6555,10 +6555,10 @@
     </row>
     <row r="109">
       <c r="A109" s="11" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="B109" s="12" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C109" s="13"/>
       <c r="D109" s="13"/>
@@ -6582,10 +6582,10 @@
     </row>
     <row r="110">
       <c r="A110" s="11" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="B110" s="12" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C110" s="13"/>
       <c r="D110" s="13"/>
@@ -6609,10 +6609,10 @@
     </row>
     <row r="111">
       <c r="A111" s="11" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="B111" s="12" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C111" s="13"/>
       <c r="D111" s="13"/>
@@ -6636,10 +6636,10 @@
     </row>
     <row r="112">
       <c r="A112" s="11" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="B112" s="12" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C112" s="13"/>
       <c r="D112" s="13"/>
@@ -6663,10 +6663,10 @@
     </row>
     <row r="113">
       <c r="A113" s="11" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="B113" s="12" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C113" s="13"/>
       <c r="D113" s="13"/>
@@ -6690,10 +6690,10 @@
     </row>
     <row r="114">
       <c r="A114" s="11" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="B114" s="12" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C114" s="13"/>
       <c r="D114" s="13"/>
@@ -6717,10 +6717,10 @@
     </row>
     <row r="115">
       <c r="A115" s="11" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="B115" s="12" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C115" s="13"/>
       <c r="D115" s="13"/>
@@ -6744,10 +6744,10 @@
     </row>
     <row r="116">
       <c r="A116" s="11" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="B116" s="12" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C116" s="13"/>
       <c r="D116" s="13"/>
@@ -6771,10 +6771,10 @@
     </row>
     <row r="117">
       <c r="A117" s="11" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="B117" s="12" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C117" s="13"/>
       <c r="D117" s="13"/>
@@ -6798,10 +6798,10 @@
     </row>
     <row r="118">
       <c r="A118" s="11" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="B118" s="12" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C118" s="13"/>
       <c r="D118" s="13"/>
@@ -6825,10 +6825,10 @@
     </row>
     <row r="119">
       <c r="A119" s="11" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="B119" s="12" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C119" s="13"/>
       <c r="D119" s="13"/>
@@ -6852,10 +6852,10 @@
     </row>
     <row r="120">
       <c r="A120" s="11" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="B120" s="12" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C120" s="13"/>
       <c r="D120" s="13"/>
@@ -6879,10 +6879,10 @@
     </row>
     <row r="121">
       <c r="A121" s="11" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="B121" s="12" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C121" s="13"/>
       <c r="D121" s="13"/>
@@ -6906,10 +6906,10 @@
     </row>
     <row r="122">
       <c r="A122" s="11" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="B122" s="12" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C122" s="13"/>
       <c r="D122" s="13"/>
@@ -6933,10 +6933,10 @@
     </row>
     <row r="123">
       <c r="A123" s="11" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="B123" s="12" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C123" s="13"/>
       <c r="D123" s="13"/>
@@ -6960,10 +6960,10 @@
     </row>
     <row r="124">
       <c r="A124" s="11" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="B124" s="12" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C124" s="13"/>
       <c r="D124" s="13"/>
@@ -6987,10 +6987,10 @@
     </row>
     <row r="125">
       <c r="A125" s="11" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="B125" s="12" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C125" s="13"/>
       <c r="D125" s="13"/>
@@ -7014,10 +7014,10 @@
     </row>
     <row r="126">
       <c r="A126" s="11" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="B126" s="12" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C126" s="13"/>
       <c r="D126" s="13"/>
@@ -7041,10 +7041,10 @@
     </row>
     <row r="127">
       <c r="A127" s="11" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="B127" s="12" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C127" s="13"/>
       <c r="D127" s="13"/>
@@ -7068,10 +7068,10 @@
     </row>
     <row r="128">
       <c r="A128" s="11" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="B128" s="12" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C128" s="13"/>
       <c r="D128" s="13"/>
@@ -7095,10 +7095,10 @@
     </row>
     <row r="129">
       <c r="A129" s="11" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="B129" s="12" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C129" s="13"/>
       <c r="D129" s="13"/>
@@ -7122,10 +7122,10 @@
     </row>
     <row r="130">
       <c r="A130" s="11" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="B130" s="12" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C130" s="13"/>
       <c r="D130" s="13"/>
@@ -7149,10 +7149,10 @@
     </row>
     <row r="131">
       <c r="A131" s="11" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="B131" s="12" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C131" s="13"/>
       <c r="D131" s="13"/>
@@ -7176,10 +7176,10 @@
     </row>
     <row r="132">
       <c r="A132" s="11" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="B132" s="12" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="C132" s="13"/>
       <c r="D132" s="13"/>
@@ -7203,10 +7203,10 @@
     </row>
     <row r="133">
       <c r="A133" s="11" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="B133" s="12" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="C133" s="13"/>
       <c r="D133" s="13"/>
@@ -7230,10 +7230,10 @@
     </row>
     <row r="134">
       <c r="A134" s="11" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="B134" s="12" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="C134" s="13"/>
       <c r="D134" s="13"/>
@@ -7257,10 +7257,10 @@
     </row>
     <row r="135">
       <c r="A135" s="11" t="s">
+        <v>147</v>
+      </c>
+      <c r="B135" s="12" t="s">
         <v>144</v>
-      </c>
-      <c r="B135" s="12" t="s">
-        <v>141</v>
       </c>
       <c r="C135" s="13"/>
       <c r="D135" s="13"/>
@@ -7284,10 +7284,10 @@
     </row>
     <row r="136">
       <c r="A136" s="11" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="B136" s="12" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="C136" s="13"/>
       <c r="D136" s="13"/>
@@ -7311,10 +7311,10 @@
     </row>
     <row r="137">
       <c r="A137" s="11" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="B137" s="12" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="C137" s="13"/>
       <c r="D137" s="13"/>
@@ -7338,10 +7338,10 @@
     </row>
     <row r="138">
       <c r="A138" s="11" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="B138" s="12" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="C138" s="13"/>
       <c r="D138" s="13"/>
@@ -7365,10 +7365,10 @@
     </row>
     <row r="139">
       <c r="A139" s="11" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="B139" s="12" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="C139" s="13"/>
       <c r="D139" s="13"/>
@@ -7392,10 +7392,10 @@
     </row>
     <row r="140">
       <c r="A140" s="11" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="B140" s="12" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="C140" s="13"/>
       <c r="D140" s="13"/>
@@ -7419,10 +7419,10 @@
     </row>
     <row r="141">
       <c r="A141" s="11" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="B141" s="12" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="C141" s="13"/>
       <c r="D141" s="13"/>
@@ -7446,10 +7446,10 @@
     </row>
     <row r="142">
       <c r="A142" s="11" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="B142" s="12" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="C142" s="13"/>
       <c r="D142" s="13"/>
@@ -7473,10 +7473,10 @@
     </row>
     <row r="143">
       <c r="A143" s="11" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="B143" s="12" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="C143" s="13"/>
       <c r="D143" s="13"/>
@@ -7500,10 +7500,10 @@
     </row>
     <row r="144">
       <c r="A144" s="11" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="B144" s="12" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="C144" s="13"/>
       <c r="D144" s="13"/>
@@ -7527,10 +7527,10 @@
     </row>
     <row r="145">
       <c r="A145" s="11" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="B145" s="12" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="C145" s="13"/>
       <c r="D145" s="13"/>
@@ -7554,10 +7554,10 @@
     </row>
     <row r="146">
       <c r="A146" s="11" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="B146" s="12" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="C146" s="13"/>
       <c r="D146" s="13"/>
@@ -7581,10 +7581,10 @@
     </row>
     <row r="147">
       <c r="A147" s="11" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="B147" s="12" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="C147" s="13"/>
       <c r="D147" s="13"/>
@@ -7608,10 +7608,10 @@
     </row>
     <row r="148">
       <c r="A148" s="11" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="B148" s="12" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="C148" s="13"/>
       <c r="D148" s="13"/>
@@ -7635,10 +7635,10 @@
     </row>
     <row r="149">
       <c r="A149" s="11" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="B149" s="12" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="C149" s="13"/>
       <c r="D149" s="13"/>
@@ -7662,10 +7662,10 @@
     </row>
     <row r="150">
       <c r="A150" s="11" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="B150" s="12" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="C150" s="13"/>
       <c r="D150" s="13"/>
@@ -7689,10 +7689,10 @@
     </row>
     <row r="151">
       <c r="A151" s="11" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="B151" s="12" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="C151" s="13"/>
       <c r="D151" s="13"/>
@@ -7716,10 +7716,10 @@
     </row>
     <row r="152">
       <c r="A152" s="11" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="B152" s="12" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="C152" s="13"/>
       <c r="D152" s="13"/>
@@ -7743,10 +7743,10 @@
     </row>
     <row r="153">
       <c r="A153" s="11" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="B153" s="12" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="C153" s="13"/>
       <c r="D153" s="13"/>
@@ -7770,10 +7770,10 @@
     </row>
     <row r="154">
       <c r="A154" s="11" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="B154" s="12" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="C154" s="13"/>
       <c r="D154" s="13"/>
@@ -7797,10 +7797,10 @@
     </row>
     <row r="155">
       <c r="A155" s="11" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="B155" s="12" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="C155" s="13"/>
       <c r="D155" s="13"/>
@@ -7824,10 +7824,10 @@
     </row>
     <row r="156">
       <c r="A156" s="11" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="B156" s="12" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="C156" s="13"/>
       <c r="D156" s="13"/>
@@ -7851,10 +7851,10 @@
     </row>
     <row r="157">
       <c r="A157" s="11" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="B157" s="12" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="C157" s="13"/>
       <c r="D157" s="13"/>
@@ -7878,10 +7878,10 @@
     </row>
     <row r="158">
       <c r="A158" s="11" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="B158" s="12" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="C158" s="13"/>
       <c r="D158" s="13"/>
@@ -7905,10 +7905,10 @@
     </row>
     <row r="159">
       <c r="A159" s="11" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="B159" s="12" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="C159" s="13"/>
       <c r="D159" s="13"/>
@@ -7932,10 +7932,10 @@
     </row>
     <row r="160">
       <c r="A160" s="11" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="B160" s="12" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="C160" s="13"/>
       <c r="D160" s="13"/>
@@ -7959,10 +7959,10 @@
     </row>
     <row r="161">
       <c r="A161" s="11" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="B161" s="12" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="C161" s="13"/>
       <c r="D161" s="13"/>
@@ -7986,10 +7986,10 @@
     </row>
     <row r="162">
       <c r="A162" s="11" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="B162" s="12" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="C162" s="13"/>
       <c r="D162" s="13"/>
@@ -8013,10 +8013,10 @@
     </row>
     <row r="163">
       <c r="A163" s="11" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="B163" s="12" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="C163" s="13"/>
       <c r="D163" s="13"/>
@@ -8040,10 +8040,10 @@
     </row>
     <row r="164">
       <c r="A164" s="11" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="B164" s="12" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="C164" s="13"/>
       <c r="D164" s="13"/>
@@ -8067,10 +8067,10 @@
     </row>
     <row r="165">
       <c r="A165" s="11" t="s">
+        <v>178</v>
+      </c>
+      <c r="B165" s="12" t="s">
         <v>175</v>
-      </c>
-      <c r="B165" s="12" t="s">
-        <v>172</v>
       </c>
       <c r="C165" s="13"/>
       <c r="D165" s="13"/>
@@ -8094,10 +8094,10 @@
     </row>
     <row r="166">
       <c r="A166" s="11" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="B166" s="12" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="C166" s="13"/>
       <c r="D166" s="13"/>
@@ -8121,10 +8121,10 @@
     </row>
     <row r="167">
       <c r="A167" s="11" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="B167" s="12" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="C167" s="13"/>
       <c r="D167" s="13"/>
@@ -8148,10 +8148,10 @@
     </row>
     <row r="168">
       <c r="A168" s="11" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="B168" s="12" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="C168" s="13"/>
       <c r="D168" s="13"/>
@@ -8175,10 +8175,10 @@
     </row>
     <row r="169">
       <c r="A169" s="11" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="B169" s="12" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="C169" s="13"/>
       <c r="D169" s="13"/>
@@ -8202,10 +8202,10 @@
     </row>
     <row r="170">
       <c r="A170" s="11" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="B170" s="12" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="C170" s="13"/>
       <c r="D170" s="13"/>
@@ -8229,10 +8229,10 @@
     </row>
     <row r="171">
       <c r="A171" s="11" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="B171" s="12" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="C171" s="13"/>
       <c r="D171" s="13"/>
@@ -8256,10 +8256,10 @@
     </row>
     <row r="172">
       <c r="A172" s="11" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="B172" s="12" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="C172" s="13"/>
       <c r="D172" s="13"/>
@@ -8283,10 +8283,10 @@
     </row>
     <row r="173">
       <c r="A173" s="11" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="B173" s="12" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="C173" s="13"/>
       <c r="D173" s="13"/>
@@ -8310,10 +8310,10 @@
     </row>
     <row r="174">
       <c r="A174" s="11" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="B174" s="12" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="C174" s="13"/>
       <c r="D174" s="13"/>
@@ -8337,10 +8337,10 @@
     </row>
     <row r="175">
       <c r="A175" s="11" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="B175" s="12" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="C175" s="13"/>
       <c r="D175" s="13"/>
@@ -8364,10 +8364,10 @@
     </row>
     <row r="176">
       <c r="A176" s="11" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="B176" s="12" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="C176" s="13"/>
       <c r="D176" s="13"/>
@@ -8391,10 +8391,10 @@
     </row>
     <row r="177">
       <c r="A177" s="11" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="B177" s="12" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="C177" s="13"/>
       <c r="D177" s="13"/>
@@ -8418,10 +8418,10 @@
     </row>
     <row r="178">
       <c r="A178" s="11" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="B178" s="12" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="C178" s="13"/>
       <c r="D178" s="13"/>
@@ -8445,10 +8445,10 @@
     </row>
     <row r="179">
       <c r="A179" s="11" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="B179" s="12" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="C179" s="13"/>
       <c r="D179" s="13"/>
@@ -8472,10 +8472,10 @@
     </row>
     <row r="180">
       <c r="A180" s="11" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="B180" s="12" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="C180" s="13"/>
       <c r="D180" s="13"/>
@@ -8499,10 +8499,10 @@
     </row>
     <row r="181">
       <c r="A181" s="11" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="B181" s="12" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="C181" s="13"/>
       <c r="D181" s="13"/>
@@ -8526,10 +8526,10 @@
     </row>
     <row r="182">
       <c r="A182" s="11" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="B182" s="12" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="C182" s="13"/>
       <c r="D182" s="13"/>
@@ -8553,10 +8553,10 @@
     </row>
     <row r="183">
       <c r="A183" s="11" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="B183" s="12" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="C183" s="13"/>
       <c r="D183" s="13"/>
@@ -8580,10 +8580,10 @@
     </row>
     <row r="184">
       <c r="A184" s="11" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="B184" s="12" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="C184" s="13"/>
       <c r="D184" s="13"/>
@@ -8607,10 +8607,10 @@
     </row>
     <row r="185">
       <c r="A185" s="11" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="B185" s="12" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="C185" s="13"/>
       <c r="D185" s="13"/>
@@ -8634,10 +8634,10 @@
     </row>
     <row r="186">
       <c r="A186" s="11" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="B186" s="12" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="C186" s="13"/>
       <c r="D186" s="13"/>
@@ -8661,10 +8661,10 @@
     </row>
     <row r="187">
       <c r="A187" s="11" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="B187" s="12" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="C187" s="13"/>
       <c r="D187" s="13"/>
@@ -8688,10 +8688,10 @@
     </row>
     <row r="188">
       <c r="A188" s="11" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="B188" s="12" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="C188" s="13"/>
       <c r="D188" s="13"/>
@@ -8715,10 +8715,10 @@
     </row>
     <row r="189">
       <c r="A189" s="11" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="B189" s="12" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="C189" s="13"/>
       <c r="D189" s="13"/>
@@ -8742,10 +8742,10 @@
     </row>
     <row r="190">
       <c r="A190" s="11" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="B190" s="12" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="C190" s="13"/>
       <c r="D190" s="13"/>
@@ -8769,10 +8769,10 @@
     </row>
     <row r="191">
       <c r="A191" s="11" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="B191" s="12" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="C191" s="13"/>
       <c r="D191" s="13"/>
@@ -8796,10 +8796,10 @@
     </row>
     <row r="192">
       <c r="A192" s="11" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="B192" s="12" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="C192" s="13"/>
       <c r="D192" s="13"/>
@@ -8823,10 +8823,10 @@
     </row>
     <row r="193">
       <c r="A193" s="11" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="B193" s="12" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="C193" s="13"/>
       <c r="D193" s="13"/>
@@ -8850,10 +8850,10 @@
     </row>
     <row r="194">
       <c r="A194" s="11" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="B194" s="12" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="C194" s="13"/>
       <c r="D194" s="13"/>
@@ -8877,10 +8877,10 @@
     </row>
     <row r="195">
       <c r="A195" s="11" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="B195" s="12" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="C195" s="13"/>
       <c r="D195" s="13"/>
@@ -8904,10 +8904,10 @@
     </row>
     <row r="196">
       <c r="A196" s="11" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="B196" s="12" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="C196" s="13"/>
       <c r="D196" s="13"/>
@@ -8931,10 +8931,10 @@
     </row>
     <row r="197">
       <c r="A197" s="11" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="B197" s="12" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="C197" s="13"/>
       <c r="D197" s="13"/>
@@ -8958,10 +8958,10 @@
     </row>
     <row r="198">
       <c r="A198" s="11" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="B198" s="12" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="C198" s="13"/>
       <c r="D198" s="13"/>
@@ -8985,10 +8985,10 @@
     </row>
     <row r="199">
       <c r="A199" s="11" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="B199" s="12" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="C199" s="13"/>
       <c r="D199" s="13"/>
@@ -9012,10 +9012,10 @@
     </row>
     <row r="200">
       <c r="A200" s="11" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="B200" s="12" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="C200" s="13"/>
       <c r="D200" s="13"/>
@@ -9039,10 +9039,10 @@
     </row>
     <row r="201">
       <c r="A201" s="11" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="B201" s="12" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="C201" s="13"/>
       <c r="D201" s="13"/>
@@ -9066,10 +9066,10 @@
     </row>
     <row r="202">
       <c r="A202" s="11" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="B202" s="12" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="C202" s="13"/>
       <c r="D202" s="13"/>
@@ -9093,10 +9093,10 @@
     </row>
     <row r="203">
       <c r="A203" s="11" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="B203" s="12" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="C203" s="13"/>
       <c r="D203" s="13"/>
@@ -9120,10 +9120,10 @@
     </row>
     <row r="204">
       <c r="A204" s="11" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="B204" s="12" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="C204" s="13"/>
       <c r="D204" s="13"/>
@@ -9147,10 +9147,10 @@
     </row>
     <row r="205">
       <c r="A205" s="11" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="B205" s="12" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="C205" s="13"/>
       <c r="D205" s="13"/>
@@ -9174,10 +9174,10 @@
     </row>
     <row r="206">
       <c r="A206" s="11" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="B206" s="12" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="C206" s="13"/>
       <c r="D206" s="13"/>
@@ -9201,10 +9201,10 @@
     </row>
     <row r="207">
       <c r="A207" s="11" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="B207" s="12" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="C207" s="13"/>
       <c r="D207" s="13"/>
@@ -9228,10 +9228,10 @@
     </row>
     <row r="208">
       <c r="A208" s="11" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="B208" s="12" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="C208" s="13"/>
       <c r="D208" s="13"/>
@@ -9255,10 +9255,10 @@
     </row>
     <row r="209">
       <c r="A209" s="11" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="B209" s="12" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="C209" s="13"/>
       <c r="D209" s="13"/>
@@ -9282,10 +9282,10 @@
     </row>
     <row r="210">
       <c r="A210" s="11" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="B210" s="12" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="C210" s="14"/>
       <c r="D210" s="13"/>
@@ -9309,10 +9309,10 @@
     </row>
     <row r="211">
       <c r="A211" s="11" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
       <c r="B211" s="12" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="C211" s="14"/>
       <c r="D211" s="15"/>
@@ -9336,10 +9336,10 @@
     </row>
     <row r="212">
       <c r="A212" s="11" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="B212" s="12" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="C212" s="14"/>
       <c r="D212" s="14"/>
@@ -9363,10 +9363,10 @@
     </row>
     <row r="213">
       <c r="A213" s="11" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="B213" s="12" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="C213" s="14"/>
       <c r="D213" s="14"/>
@@ -9390,10 +9390,10 @@
     </row>
     <row r="214">
       <c r="A214" s="11" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
       <c r="B214" s="12" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="C214" s="14"/>
       <c r="D214" s="14"/>
@@ -9417,10 +9417,10 @@
     </row>
     <row r="215">
       <c r="A215" s="11" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
       <c r="B215" s="12" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="C215" s="14"/>
       <c r="D215" s="14"/>
@@ -9444,10 +9444,10 @@
     </row>
     <row r="216">
       <c r="A216" s="11" t="s">
-        <v>226</v>
+        <v>229</v>
       </c>
       <c r="B216" s="12" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="C216" s="14"/>
       <c r="D216" s="14"/>
@@ -9471,10 +9471,10 @@
     </row>
     <row r="217">
       <c r="A217" s="11" t="s">
-        <v>227</v>
+        <v>230</v>
       </c>
       <c r="B217" s="12" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="C217" s="14"/>
       <c r="D217" s="14"/>
@@ -9498,10 +9498,10 @@
     </row>
     <row r="218">
       <c r="A218" s="11" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
       <c r="B218" s="12" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="C218" s="14"/>
       <c r="D218" s="14"/>
@@ -9525,10 +9525,10 @@
     </row>
     <row r="219">
       <c r="A219" s="11" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
       <c r="B219" s="12" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="C219" s="14"/>
       <c r="D219" s="14"/>
@@ -9552,10 +9552,10 @@
     </row>
     <row r="220">
       <c r="A220" s="11" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
       <c r="B220" s="12" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="C220" s="14"/>
       <c r="D220" s="14"/>
@@ -9579,10 +9579,10 @@
     </row>
     <row r="221">
       <c r="A221" s="11" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="B221" s="12" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="C221" s="14"/>
       <c r="D221" s="14"/>
@@ -9606,10 +9606,10 @@
     </row>
     <row r="222">
       <c r="A222" s="11" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="B222" s="12" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="C222" s="14"/>
       <c r="D222" s="14"/>
@@ -9633,10 +9633,10 @@
     </row>
     <row r="223">
       <c r="A223" s="11" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
       <c r="B223" s="12" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="C223" s="14"/>
       <c r="D223" s="14"/>
@@ -9660,10 +9660,10 @@
     </row>
     <row r="224">
       <c r="A224" s="11" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
       <c r="B224" s="12" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="C224" s="14"/>
       <c r="D224" s="14"/>
@@ -9687,10 +9687,10 @@
     </row>
     <row r="225">
       <c r="A225" s="11" t="s">
-        <v>235</v>
+        <v>238</v>
       </c>
       <c r="B225" s="12" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="C225" s="14"/>
       <c r="D225" s="14"/>
@@ -9714,10 +9714,10 @@
     </row>
     <row r="226">
       <c r="A226" s="11" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="B226" s="12" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="C226" s="14"/>
       <c r="D226" s="14"/>
@@ -9741,10 +9741,10 @@
     </row>
     <row r="227">
       <c r="A227" s="11" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
       <c r="B227" s="12" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="C227" s="14"/>
       <c r="D227" s="16"/>
@@ -9768,10 +9768,10 @@
     </row>
     <row r="228">
       <c r="A228" s="11" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="B228" s="12" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="C228" s="14"/>
       <c r="D228" s="14"/>
@@ -9795,10 +9795,10 @@
     </row>
     <row r="229">
       <c r="A229" s="11" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="B229" s="12" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="C229" s="14"/>
       <c r="D229" s="14"/>
@@ -9822,10 +9822,10 @@
     </row>
     <row r="230">
       <c r="A230" s="11" t="s">
-        <v>240</v>
+        <v>243</v>
       </c>
       <c r="B230" s="12" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="C230" s="14"/>
       <c r="D230" s="14"/>
@@ -9849,10 +9849,10 @@
     </row>
     <row r="231">
       <c r="A231" s="11" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="B231" s="12" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="C231" s="14"/>
       <c r="D231" s="14"/>
@@ -9876,10 +9876,10 @@
     </row>
     <row r="232">
       <c r="A232" s="11" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
       <c r="B232" s="12" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="C232" s="14"/>
       <c r="D232" s="14"/>
@@ -9903,10 +9903,10 @@
     </row>
     <row r="233">
       <c r="A233" s="11" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
       <c r="B233" s="12" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="C233" s="14"/>
       <c r="D233" s="14"/>
@@ -9930,10 +9930,10 @@
     </row>
     <row r="234">
       <c r="A234" s="11" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
       <c r="B234" s="12" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="C234" s="14"/>
       <c r="D234" s="14"/>
@@ -9957,10 +9957,10 @@
     </row>
     <row r="235">
       <c r="A235" s="11" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="B235" s="12" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="C235" s="14"/>
       <c r="D235" s="14"/>
@@ -9984,10 +9984,10 @@
     </row>
     <row r="236">
       <c r="A236" s="11" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
       <c r="B236" s="12" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="C236" s="14"/>
       <c r="D236" s="14"/>
@@ -10011,10 +10011,10 @@
     </row>
     <row r="237">
       <c r="A237" s="11" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
       <c r="B237" s="12" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="C237" s="14"/>
       <c r="D237" s="14"/>
@@ -10038,10 +10038,10 @@
     </row>
     <row r="238">
       <c r="A238" s="11" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="B238" s="12" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="C238" s="14"/>
       <c r="D238" s="14"/>
@@ -10065,10 +10065,10 @@
     </row>
     <row r="239">
       <c r="A239" s="11" t="s">
-        <v>249</v>
+        <v>252</v>
       </c>
       <c r="B239" s="12" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="C239" s="14"/>
       <c r="D239" s="14"/>
@@ -10092,10 +10092,10 @@
     </row>
     <row r="240">
       <c r="A240" s="11" t="s">
-        <v>250</v>
+        <v>253</v>
       </c>
       <c r="B240" s="12" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="C240" s="14"/>
       <c r="D240" s="14"/>
@@ -10119,10 +10119,10 @@
     </row>
     <row r="241">
       <c r="A241" s="11" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="B241" s="12" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="C241" s="14"/>
       <c r="D241" s="14"/>
@@ -10146,10 +10146,10 @@
     </row>
     <row r="242">
       <c r="A242" s="11" t="s">
-        <v>252</v>
+        <v>255</v>
       </c>
       <c r="B242" s="12" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="C242" s="14"/>
       <c r="D242" s="13"/>
@@ -10173,10 +10173,10 @@
     </row>
     <row r="243">
       <c r="A243" s="11" t="s">
-        <v>253</v>
+        <v>256</v>
       </c>
       <c r="B243" s="12" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="C243" s="14"/>
       <c r="D243" s="15"/>
@@ -10200,10 +10200,10 @@
     </row>
     <row r="244">
       <c r="A244" s="11" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
       <c r="B244" s="12" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="C244" s="14"/>
       <c r="D244" s="14"/>
@@ -10227,10 +10227,10 @@
     </row>
     <row r="245">
       <c r="A245" s="11" t="s">
-        <v>255</v>
+        <v>258</v>
       </c>
       <c r="B245" s="12" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="C245" s="14"/>
       <c r="D245" s="14"/>
@@ -10254,10 +10254,10 @@
     </row>
     <row r="246">
       <c r="A246" s="11" t="s">
-        <v>256</v>
+        <v>259</v>
       </c>
       <c r="B246" s="12" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="C246" s="14"/>
       <c r="D246" s="14"/>
@@ -10281,10 +10281,10 @@
     </row>
     <row r="247">
       <c r="A247" s="11" t="s">
-        <v>257</v>
+        <v>260</v>
       </c>
       <c r="B247" s="12" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="C247" s="14"/>
       <c r="D247" s="14"/>
@@ -10308,10 +10308,10 @@
     </row>
     <row r="248">
       <c r="A248" s="11" t="s">
-        <v>258</v>
+        <v>261</v>
       </c>
       <c r="B248" s="12" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="C248" s="14"/>
       <c r="D248" s="14"/>
@@ -10335,10 +10335,10 @@
     </row>
     <row r="249">
       <c r="A249" s="11" t="s">
-        <v>259</v>
+        <v>262</v>
       </c>
       <c r="B249" s="12" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="C249" s="14"/>
       <c r="D249" s="14"/>
@@ -10362,10 +10362,10 @@
     </row>
     <row r="250">
       <c r="A250" s="11" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
       <c r="B250" s="12" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="C250" s="14"/>
       <c r="D250" s="14"/>
@@ -10389,10 +10389,10 @@
     </row>
     <row r="251">
       <c r="A251" s="11" t="s">
-        <v>261</v>
+        <v>264</v>
       </c>
       <c r="B251" s="12" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="C251" s="14"/>
       <c r="D251" s="14"/>
@@ -10416,10 +10416,10 @@
     </row>
     <row r="252">
       <c r="A252" s="11" t="s">
-        <v>262</v>
+        <v>265</v>
       </c>
       <c r="B252" s="12" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="C252" s="14"/>
       <c r="D252" s="14"/>
@@ -10443,10 +10443,10 @@
     </row>
     <row r="253">
       <c r="A253" s="11" t="s">
-        <v>263</v>
+        <v>266</v>
       </c>
       <c r="B253" s="12" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="C253" s="14"/>
       <c r="D253" s="14"/>
@@ -10470,10 +10470,10 @@
     </row>
     <row r="254">
       <c r="A254" s="11" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
       <c r="B254" s="12" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="C254" s="14"/>
       <c r="D254" s="14"/>
@@ -10497,10 +10497,10 @@
     </row>
     <row r="255">
       <c r="A255" s="11" t="s">
-        <v>265</v>
+        <v>268</v>
       </c>
       <c r="B255" s="12" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="C255" s="14"/>
       <c r="D255" s="14"/>
@@ -10524,10 +10524,10 @@
     </row>
     <row r="256">
       <c r="A256" s="11" t="s">
-        <v>266</v>
+        <v>269</v>
       </c>
       <c r="B256" s="12" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="C256" s="14"/>
       <c r="D256" s="14"/>
@@ -10551,10 +10551,10 @@
     </row>
     <row r="257">
       <c r="A257" s="11" t="s">
-        <v>267</v>
+        <v>270</v>
       </c>
       <c r="B257" s="12" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="C257" s="4"/>
       <c r="D257" s="4"/>
@@ -10578,10 +10578,10 @@
     </row>
     <row r="258">
       <c r="A258" s="11" t="s">
-        <v>268</v>
+        <v>271</v>
       </c>
       <c r="B258" s="12" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="C258" s="4"/>
       <c r="D258" s="4"/>
@@ -10605,10 +10605,10 @@
     </row>
     <row r="259">
       <c r="A259" s="11" t="s">
-        <v>269</v>
+        <v>272</v>
       </c>
       <c r="B259" s="12" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="C259" s="4"/>
       <c r="D259" s="4"/>
@@ -10632,10 +10632,10 @@
     </row>
     <row r="260">
       <c r="A260" s="11" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="B260" s="12" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="C260" s="4"/>
       <c r="D260" s="4"/>
@@ -10659,10 +10659,10 @@
     </row>
     <row r="261">
       <c r="A261" s="17" t="s">
-        <v>271</v>
+        <v>274</v>
       </c>
       <c r="B261" s="17" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="C261" s="5"/>
       <c r="D261" s="5"/>
@@ -10704,7 +10704,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="2" t="s">
-        <v>272</v>
+        <v>8</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -13300,10 +13300,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="2" t="s">
-        <v>273</v>
+        <v>109</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>274</v>
+        <v>110</v>
       </c>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>

</xml_diff>